<commit_message>
Added for loop to main file for calculating Full Covid-19 Mortality PYLL to adjust for 2020-2021 periods.
Signed-off-by: Mlad-en <mmladenov1992@gmail.com>
</commit_message>
<xml_diff>
--- a/data_source/InfoStat - Cleaned/en_infostat_life_expectancy_by_sex.xlsx
+++ b/data_source/InfoStat - Cleaned/en_infostat_life_expectancy_by_sex.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524" uniqueCount="231">
   <si>
     <t/>
   </si>
@@ -26,28 +26,46 @@
     <t>5703:2017 - 2019:5</t>
   </si>
   <si>
+    <t>2018 - 2020</t>
+  </si>
+  <si>
+    <t>5703:2018 - 2020:6</t>
+  </si>
+  <si>
     <t>Life expectancy</t>
   </si>
   <si>
-    <t>5703:2017 - 2019:5;5702:1.1.3.1:24</t>
+    <t>5703:2017 - 2019:5;5702:1.1.3.1:25</t>
+  </si>
+  <si>
+    <t>5703:2018 - 2020:6;5702:1.1.3.1:25</t>
   </si>
   <si>
     <t>Total</t>
   </si>
   <si>
-    <t>5703:2017 - 2019:5;5702:1.1.3.1:24;5701:0:0</t>
+    <t>5703:2017 - 2019:5;5702:1.1.3.1:25;5701:0:0</t>
   </si>
   <si>
     <t>Male</t>
   </si>
   <si>
-    <t>5703:2017 - 2019:5;5702:1.1.3.1:24;5701:1:2</t>
+    <t>5703:2017 - 2019:5;5702:1.1.3.1:25;5701:1:2</t>
   </si>
   <si>
     <t>Female</t>
   </si>
   <si>
-    <t>5703:2017 - 2019:5;5702:1.1.3.1:24;5701:2:3</t>
+    <t>5703:2017 - 2019:5;5702:1.1.3.1:25;5701:2:3</t>
+  </si>
+  <si>
+    <t>5703:2018 - 2020:6;5702:1.1.3.1:25;5701:0:0</t>
+  </si>
+  <si>
+    <t>5703:2018 - 2020:6;5702:1.1.3.1:25;5701:1:2</t>
+  </si>
+  <si>
+    <t>5703:2018 - 2020:6;5702:1.1.3.1:25;5701:2:3</t>
   </si>
   <si>
     <t>5704:0:1</t>
@@ -62,601 +80,601 @@
     <t>1</t>
   </si>
   <si>
-    <t>5704:0:15700:1:6</t>
+    <t>5704:0:15700:1:7</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
-    <t>5704:0:15700:2:7</t>
+    <t>5704:0:15700:2:8</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>5704:0:15700:3:8</t>
+    <t>5704:0:15700:3:9</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
-    <t>5704:0:15700:4:9</t>
+    <t>5704:0:15700:4:10</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
-    <t>5704:0:15700:5:10</t>
+    <t>5704:0:15700:5:11</t>
   </si>
   <si>
     <t>6</t>
   </si>
   <si>
-    <t>5704:0:15700:6:11</t>
+    <t>5704:0:15700:6:12</t>
   </si>
   <si>
     <t>7</t>
   </si>
   <si>
-    <t>5704:0:15700:7:12</t>
+    <t>5704:0:15700:7:13</t>
   </si>
   <si>
     <t>8</t>
   </si>
   <si>
-    <t>5704:0:15700:8:13</t>
+    <t>5704:0:15700:8:14</t>
   </si>
   <si>
     <t>9</t>
   </si>
   <si>
-    <t>5704:0:15700:9:14</t>
+    <t>5704:0:15700:9:15</t>
   </si>
   <si>
     <t>10</t>
   </si>
   <si>
-    <t>5704:0:15700:10:15</t>
+    <t>5704:0:15700:10:16</t>
   </si>
   <si>
     <t>11</t>
   </si>
   <si>
-    <t>5704:0:15700:11:16</t>
+    <t>5704:0:15700:11:17</t>
   </si>
   <si>
     <t>12</t>
   </si>
   <si>
-    <t>5704:0:15700:12:17</t>
+    <t>5704:0:15700:12:18</t>
   </si>
   <si>
     <t>13</t>
   </si>
   <si>
-    <t>5704:0:15700:13:18</t>
+    <t>5704:0:15700:13:19</t>
   </si>
   <si>
     <t>14</t>
   </si>
   <si>
-    <t>5704:0:15700:14:19</t>
+    <t>5704:0:15700:14:20</t>
   </si>
   <si>
     <t>15</t>
   </si>
   <si>
-    <t>5704:0:15700:15:20</t>
+    <t>5704:0:15700:15:21</t>
   </si>
   <si>
     <t>16</t>
   </si>
   <si>
-    <t>5704:0:15700:16:21</t>
+    <t>5704:0:15700:16:22</t>
   </si>
   <si>
     <t>17</t>
   </si>
   <si>
-    <t>5704:0:15700:17:22</t>
+    <t>5704:0:15700:17:23</t>
   </si>
   <si>
     <t>18</t>
   </si>
   <si>
-    <t>5704:0:15700:18:23</t>
+    <t>5704:0:15700:18:24</t>
   </si>
   <si>
     <t>19</t>
   </si>
   <si>
-    <t>5704:0:15700:19:25</t>
+    <t>5704:0:15700:19:26</t>
   </si>
   <si>
     <t>20</t>
   </si>
   <si>
-    <t>5704:0:15700:20:26</t>
+    <t>5704:0:15700:20:27</t>
   </si>
   <si>
     <t>21</t>
   </si>
   <si>
-    <t>5704:0:15700:21:27</t>
+    <t>5704:0:15700:21:28</t>
   </si>
   <si>
     <t>22</t>
   </si>
   <si>
-    <t>5704:0:15700:22:28</t>
+    <t>5704:0:15700:22:29</t>
   </si>
   <si>
     <t>23</t>
   </si>
   <si>
-    <t>5704:0:15700:23:29</t>
+    <t>5704:0:15700:23:30</t>
   </si>
   <si>
     <t>24</t>
   </si>
   <si>
-    <t>5704:0:15700:24:30</t>
+    <t>5704:0:15700:24:31</t>
   </si>
   <si>
     <t>25</t>
   </si>
   <si>
-    <t>5704:0:15700:25:31</t>
+    <t>5704:0:15700:25:32</t>
   </si>
   <si>
     <t>26</t>
   </si>
   <si>
-    <t>5704:0:15700:26:32</t>
+    <t>5704:0:15700:26:33</t>
   </si>
   <si>
     <t>27</t>
   </si>
   <si>
-    <t>5704:0:15700:27:33</t>
+    <t>5704:0:15700:27:34</t>
   </si>
   <si>
     <t>28</t>
   </si>
   <si>
-    <t>5704:0:15700:28:34</t>
+    <t>5704:0:15700:28:35</t>
   </si>
   <si>
     <t>29</t>
   </si>
   <si>
-    <t>5704:0:15700:29:35</t>
+    <t>5704:0:15700:29:36</t>
   </si>
   <si>
     <t>30</t>
   </si>
   <si>
-    <t>5704:0:15700:30:36</t>
+    <t>5704:0:15700:30:37</t>
   </si>
   <si>
     <t>31</t>
   </si>
   <si>
-    <t>5704:0:15700:31:37</t>
+    <t>5704:0:15700:31:38</t>
   </si>
   <si>
     <t>32</t>
   </si>
   <si>
-    <t>5704:0:15700:32:38</t>
+    <t>5704:0:15700:32:39</t>
   </si>
   <si>
     <t>33</t>
   </si>
   <si>
-    <t>5704:0:15700:33:39</t>
+    <t>5704:0:15700:33:40</t>
   </si>
   <si>
     <t>34</t>
   </si>
   <si>
-    <t>5704:0:15700:34:40</t>
+    <t>5704:0:15700:34:41</t>
   </si>
   <si>
     <t>35</t>
   </si>
   <si>
-    <t>5704:0:15700:35:41</t>
+    <t>5704:0:15700:35:42</t>
   </si>
   <si>
     <t>36</t>
   </si>
   <si>
-    <t>5704:0:15700:36:42</t>
+    <t>5704:0:15700:36:43</t>
   </si>
   <si>
     <t>37</t>
   </si>
   <si>
-    <t>5704:0:15700:37:43</t>
+    <t>5704:0:15700:37:44</t>
   </si>
   <si>
     <t>38</t>
   </si>
   <si>
-    <t>5704:0:15700:38:44</t>
+    <t>5704:0:15700:38:45</t>
   </si>
   <si>
     <t>39</t>
   </si>
   <si>
-    <t>5704:0:15700:39:45</t>
+    <t>5704:0:15700:39:46</t>
   </si>
   <si>
     <t>40</t>
   </si>
   <si>
-    <t>5704:0:15700:40:46</t>
+    <t>5704:0:15700:40:47</t>
   </si>
   <si>
     <t>41</t>
   </si>
   <si>
-    <t>5704:0:15700:41:47</t>
+    <t>5704:0:15700:41:48</t>
   </si>
   <si>
     <t>42</t>
   </si>
   <si>
-    <t>5704:0:15700:42:48</t>
+    <t>5704:0:15700:42:49</t>
   </si>
   <si>
     <t>43</t>
   </si>
   <si>
-    <t>5704:0:15700:43:49</t>
+    <t>5704:0:15700:43:50</t>
   </si>
   <si>
     <t>44</t>
   </si>
   <si>
-    <t>5704:0:15700:44:50</t>
+    <t>5704:0:15700:44:51</t>
   </si>
   <si>
     <t>45</t>
   </si>
   <si>
-    <t>5704:0:15700:45:51</t>
+    <t>5704:0:15700:45:52</t>
   </si>
   <si>
     <t>46</t>
   </si>
   <si>
-    <t>5704:0:15700:46:52</t>
+    <t>5704:0:15700:46:53</t>
   </si>
   <si>
     <t>47</t>
   </si>
   <si>
-    <t>5704:0:15700:47:53</t>
+    <t>5704:0:15700:47:54</t>
   </si>
   <si>
     <t>48</t>
   </si>
   <si>
-    <t>5704:0:15700:48:54</t>
+    <t>5704:0:15700:48:55</t>
   </si>
   <si>
     <t>49</t>
   </si>
   <si>
-    <t>5704:0:15700:49:55</t>
+    <t>5704:0:15700:49:56</t>
   </si>
   <si>
     <t>50</t>
   </si>
   <si>
-    <t>5704:0:15700:50:56</t>
+    <t>5704:0:15700:50:57</t>
   </si>
   <si>
     <t>51</t>
   </si>
   <si>
-    <t>5704:0:15700:51:57</t>
+    <t>5704:0:15700:51:58</t>
   </si>
   <si>
     <t>52</t>
   </si>
   <si>
-    <t>5704:0:15700:52:58</t>
+    <t>5704:0:15700:52:59</t>
   </si>
   <si>
     <t>53</t>
   </si>
   <si>
-    <t>5704:0:15700:53:59</t>
+    <t>5704:0:15700:53:60</t>
   </si>
   <si>
     <t>54</t>
   </si>
   <si>
-    <t>5704:0:15700:54:60</t>
+    <t>5704:0:15700:54:61</t>
   </si>
   <si>
     <t>55</t>
   </si>
   <si>
-    <t>5704:0:15700:55:61</t>
+    <t>5704:0:15700:55:62</t>
   </si>
   <si>
     <t>56</t>
   </si>
   <si>
-    <t>5704:0:15700:56:62</t>
+    <t>5704:0:15700:56:63</t>
   </si>
   <si>
     <t>57</t>
   </si>
   <si>
-    <t>5704:0:15700:57:63</t>
+    <t>5704:0:15700:57:64</t>
   </si>
   <si>
     <t>58</t>
   </si>
   <si>
-    <t>5704:0:15700:58:64</t>
+    <t>5704:0:15700:58:65</t>
   </si>
   <si>
     <t>59</t>
   </si>
   <si>
-    <t>5704:0:15700:59:65</t>
+    <t>5704:0:15700:59:66</t>
   </si>
   <si>
     <t>60</t>
   </si>
   <si>
-    <t>5704:0:15700:60:66</t>
+    <t>5704:0:15700:60:67</t>
   </si>
   <si>
     <t>61</t>
   </si>
   <si>
-    <t>5704:0:15700:61:67</t>
+    <t>5704:0:15700:61:68</t>
   </si>
   <si>
     <t>62</t>
   </si>
   <si>
-    <t>5704:0:15700:62:68</t>
+    <t>5704:0:15700:62:69</t>
   </si>
   <si>
     <t>63</t>
   </si>
   <si>
-    <t>5704:0:15700:63:69</t>
+    <t>5704:0:15700:63:70</t>
   </si>
   <si>
     <t>64</t>
   </si>
   <si>
-    <t>5704:0:15700:64:70</t>
+    <t>5704:0:15700:64:71</t>
   </si>
   <si>
     <t>65</t>
   </si>
   <si>
-    <t>5704:0:15700:65:71</t>
+    <t>5704:0:15700:65:72</t>
   </si>
   <si>
     <t>66</t>
   </si>
   <si>
-    <t>5704:0:15700:66:72</t>
+    <t>5704:0:15700:66:73</t>
   </si>
   <si>
     <t>67</t>
   </si>
   <si>
-    <t>5704:0:15700:67:73</t>
+    <t>5704:0:15700:67:74</t>
   </si>
   <si>
     <t>68</t>
   </si>
   <si>
-    <t>5704:0:15700:68:74</t>
+    <t>5704:0:15700:68:75</t>
   </si>
   <si>
     <t>69</t>
   </si>
   <si>
-    <t>5704:0:15700:69:75</t>
+    <t>5704:0:15700:69:76</t>
   </si>
   <si>
     <t>70</t>
   </si>
   <si>
-    <t>5704:0:15700:70:76</t>
+    <t>5704:0:15700:70:77</t>
   </si>
   <si>
     <t>71</t>
   </si>
   <si>
-    <t>5704:0:15700:71:77</t>
+    <t>5704:0:15700:71:78</t>
   </si>
   <si>
     <t>72</t>
   </si>
   <si>
-    <t>5704:0:15700:72:78</t>
+    <t>5704:0:15700:72:79</t>
   </si>
   <si>
     <t>73</t>
   </si>
   <si>
-    <t>5704:0:15700:73:79</t>
+    <t>5704:0:15700:73:80</t>
   </si>
   <si>
     <t>74</t>
   </si>
   <si>
-    <t>5704:0:15700:74:80</t>
+    <t>5704:0:15700:74:81</t>
   </si>
   <si>
     <t>75</t>
   </si>
   <si>
-    <t>5704:0:15700:75:81</t>
+    <t>5704:0:15700:75:82</t>
   </si>
   <si>
     <t>76</t>
   </si>
   <si>
-    <t>5704:0:15700:76:82</t>
+    <t>5704:0:15700:76:83</t>
   </si>
   <si>
     <t>77</t>
   </si>
   <si>
-    <t>5704:0:15700:77:83</t>
+    <t>5704:0:15700:77:84</t>
   </si>
   <si>
     <t>78</t>
   </si>
   <si>
-    <t>5704:0:15700:78:84</t>
+    <t>5704:0:15700:78:85</t>
   </si>
   <si>
     <t>79</t>
   </si>
   <si>
-    <t>5704:0:15700:79:85</t>
+    <t>5704:0:15700:79:86</t>
   </si>
   <si>
     <t>80</t>
   </si>
   <si>
-    <t>5704:0:15700:80:86</t>
+    <t>5704:0:15700:80:87</t>
   </si>
   <si>
     <t>81</t>
   </si>
   <si>
-    <t>5704:0:15700:81:87</t>
+    <t>5704:0:15700:81:88</t>
   </si>
   <si>
     <t>82</t>
   </si>
   <si>
-    <t>5704:0:15700:82:88</t>
+    <t>5704:0:15700:82:89</t>
   </si>
   <si>
     <t>83</t>
   </si>
   <si>
-    <t>5704:0:15700:83:89</t>
+    <t>5704:0:15700:83:90</t>
   </si>
   <si>
     <t>84</t>
   </si>
   <si>
-    <t>5704:0:15700:84:90</t>
+    <t>5704:0:15700:84:91</t>
   </si>
   <si>
     <t>85</t>
   </si>
   <si>
-    <t>5704:0:15700:85:91</t>
+    <t>5704:0:15700:85:92</t>
   </si>
   <si>
     <t>86</t>
   </si>
   <si>
-    <t>5704:0:15700:86:92</t>
+    <t>5704:0:15700:86:93</t>
   </si>
   <si>
     <t>87</t>
   </si>
   <si>
-    <t>5704:0:15700:87:93</t>
+    <t>5704:0:15700:87:94</t>
   </si>
   <si>
     <t>88</t>
   </si>
   <si>
-    <t>5704:0:15700:88:94</t>
+    <t>5704:0:15700:88:95</t>
   </si>
   <si>
     <t>89</t>
   </si>
   <si>
-    <t>5704:0:15700:89:95</t>
+    <t>5704:0:15700:89:96</t>
   </si>
   <si>
     <t>90</t>
   </si>
   <si>
-    <t>5704:0:15700:90:96</t>
+    <t>5704:0:15700:90:97</t>
   </si>
   <si>
     <t>91</t>
   </si>
   <si>
-    <t>5704:0:15700:91:97</t>
+    <t>5704:0:15700:91:98</t>
   </si>
   <si>
     <t>92</t>
   </si>
   <si>
-    <t>5704:0:15700:92:98</t>
+    <t>5704:0:15700:92:99</t>
   </si>
   <si>
     <t>93</t>
   </si>
   <si>
-    <t>5704:0:15700:93:99</t>
+    <t>5704:0:15700:93:100</t>
   </si>
   <si>
     <t>94</t>
   </si>
   <si>
-    <t>5704:0:15700:94:100</t>
+    <t>5704:0:15700:94:101</t>
   </si>
   <si>
     <t>95</t>
   </si>
   <si>
-    <t>5704:0:15700:95:101</t>
+    <t>5704:0:15700:95:102</t>
   </si>
   <si>
     <t>96</t>
   </si>
   <si>
-    <t>5704:0:15700:96:102</t>
+    <t>5704:0:15700:96:103</t>
   </si>
   <si>
     <t>97</t>
   </si>
   <si>
-    <t>5704:0:15700:97:103</t>
+    <t>5704:0:15700:97:104</t>
   </si>
   <si>
     <t>98</t>
   </si>
   <si>
-    <t>5704:0:15700:98:104</t>
+    <t>5704:0:15700:98:105</t>
   </si>
   <si>
     <t>99</t>
   </si>
   <si>
-    <t>5704:0:15700:99:105</t>
+    <t>5704:0:15700:99:106</t>
   </si>
   <si>
     <t>100+</t>
   </si>
   <si>
-    <t>5704:0:15700:100+:106</t>
+    <t>5704:0:15700:100+:107</t>
   </si>
   <si>
     <t>Notes</t>
@@ -686,7 +704,7 @@
     <t>Age</t>
   </si>
   <si>
-    <t>Date of preparation of inquiry 03/05/2021</t>
+    <t>Date of preparation of inquiry 18/05/2021</t>
   </si>
 </sst>
 </file>
@@ -974,6 +992,9 @@
     <col min="3" max="3" width="11.0" customWidth="true"/>
     <col min="4" max="4" width="11.0" customWidth="true"/>
     <col min="5" max="5" width="11.0" customWidth="true"/>
+    <col min="6" max="6" width="11.0" customWidth="true"/>
+    <col min="7" max="7" width="11.0" customWidth="true"/>
+    <col min="8" max="8" width="11.0" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -997,6 +1018,15 @@
       <c r="E2" t="s" s="8">
         <v>2</v>
       </c>
+      <c r="F2" t="s" s="8">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s" s="8">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s" s="8">
+        <v>4</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="7">
@@ -1006,13 +1036,22 @@
         <v>0</v>
       </c>
       <c r="C3" t="s" s="9">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s" s="9">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s" s="9">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="F3" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s" s="9">
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -1023,21 +1062,30 @@
         <v>0</v>
       </c>
       <c r="C4" t="s" s="10">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s" s="10">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s" s="10">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="F4" t="s" s="10">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s" s="10">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s" s="10">
+        <v>13</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s" s="12">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C5" t="n" s="13">
         <v>74.90475343548141</v>
@@ -1048,13 +1096,22 @@
       <c r="E5" t="n" s="13">
         <v>78.45429921233465</v>
       </c>
+      <c r="F5" t="n" s="13">
+        <v>74.63778958961784</v>
+      </c>
+      <c r="G5" t="n" s="13">
+        <v>71.10716604870449</v>
+      </c>
+      <c r="H5" t="n" s="13">
+        <v>78.21909304438181</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s" s="12">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C6" t="n" s="14">
         <v>74.35189422464101</v>
@@ -1065,13 +1122,22 @@
       <c r="E6" t="n" s="14">
         <v>77.89725664031499</v>
       </c>
+      <c r="F6" t="n" s="14">
+        <v>74.04860759971515</v>
+      </c>
+      <c r="G6" t="n" s="14">
+        <v>70.5403922979688</v>
+      </c>
+      <c r="H6" t="n" s="14">
+        <v>77.60130068847258</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s" s="12">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C7" t="n" s="13">
         <v>73.38902090134329</v>
@@ -1082,13 +1148,22 @@
       <c r="E7" t="n" s="13">
         <v>76.9516392785562</v>
       </c>
+      <c r="F7" t="n" s="13">
+        <v>73.07572511215629</v>
+      </c>
+      <c r="G7" t="n" s="13">
+        <v>69.56538460620496</v>
+      </c>
+      <c r="H7" t="n" s="13">
+        <v>76.63073416866182</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s" s="12">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C8" t="n" s="14">
         <v>72.41742902764703</v>
@@ -1099,13 +1174,22 @@
       <c r="E8" t="n" s="14">
         <v>75.99000970994149</v>
       </c>
+      <c r="F8" t="n" s="14">
+        <v>72.09991775969387</v>
+      </c>
+      <c r="G8" t="n" s="14">
+        <v>68.58333741891357</v>
+      </c>
+      <c r="H8" t="n" s="14">
+        <v>75.66199839535501</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s" s="12">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C9" t="n" s="13">
         <v>71.43850954470544</v>
@@ -1116,13 +1200,22 @@
       <c r="E9" t="n" s="13">
         <v>75.0177973685409</v>
       </c>
+      <c r="F9" t="n" s="13">
+        <v>71.12130191977867</v>
+      </c>
+      <c r="G9" t="n" s="13">
+        <v>67.60771646197881</v>
+      </c>
+      <c r="H9" t="n" s="13">
+        <v>74.67971503397793</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s" s="12">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C10" t="n" s="14">
         <v>70.45697423564651</v>
@@ -1133,13 +1226,22 @@
       <c r="E10" t="n" s="14">
         <v>74.0377434612896</v>
       </c>
+      <c r="F10" t="n" s="14">
+        <v>70.13076552540313</v>
+      </c>
+      <c r="G10" t="n" s="14">
+        <v>66.61865967307534</v>
+      </c>
+      <c r="H10" t="n" s="14">
+        <v>73.68738584639836</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s" s="12">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C11" t="n" s="13">
         <v>69.47169707994597</v>
@@ -1150,13 +1252,22 @@
       <c r="E11" t="n" s="13">
         <v>73.04681643649536</v>
       </c>
+      <c r="F11" t="n" s="13">
+        <v>69.14066199943457</v>
+      </c>
+      <c r="G11" t="n" s="13">
+        <v>65.62925665181533</v>
+      </c>
+      <c r="H11" t="n" s="13">
+        <v>72.6963865255642</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s" s="12">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C12" t="n" s="14">
         <v>68.4808917141519</v>
@@ -1167,13 +1278,22 @@
       <c r="E12" t="n" s="14">
         <v>72.05899294514224</v>
       </c>
+      <c r="F12" t="n" s="14">
+        <v>68.14889381340583</v>
+      </c>
+      <c r="G12" t="n" s="14">
+        <v>64.6368740616106</v>
+      </c>
+      <c r="H12" t="n" s="14">
+        <v>71.70527023752437</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s" s="12">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C13" t="n" s="13">
         <v>67.49718619552685</v>
@@ -1184,13 +1304,22 @@
       <c r="E13" t="n" s="13">
         <v>71.07508692093963</v>
       </c>
+      <c r="F13" t="n" s="13">
+        <v>67.16090446415988</v>
+      </c>
+      <c r="G13" t="n" s="13">
+        <v>63.64885650025162</v>
+      </c>
+      <c r="H13" t="n" s="13">
+        <v>70.71721117598545</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s" s="12">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C14" t="n" s="14">
         <v>66.50529584342031</v>
@@ -1201,13 +1330,22 @@
       <c r="E14" t="n" s="14">
         <v>70.0870785985348</v>
       </c>
+      <c r="F14" t="n" s="14">
+        <v>66.16816607036564</v>
+      </c>
+      <c r="G14" t="n" s="14">
+        <v>62.65597342509107</v>
+      </c>
+      <c r="H14" t="n" s="14">
+        <v>69.7245788133094</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s" s="12">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C15" t="n" s="13">
         <v>65.5150023800072</v>
@@ -1218,13 +1356,22 @@
       <c r="E15" t="n" s="13">
         <v>69.09506982345617</v>
       </c>
+      <c r="F15" t="n" s="13">
+        <v>65.17751566895116</v>
+      </c>
+      <c r="G15" t="n" s="13">
+        <v>61.66286705087798</v>
+      </c>
+      <c r="H15" t="n" s="13">
+        <v>68.73673283034829</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s" s="12">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C16" t="n" s="14">
         <v>64.52333042175562</v>
@@ -1235,13 +1382,22 @@
       <c r="E16" t="n" s="14">
         <v>68.10209626383106</v>
       </c>
+      <c r="F16" t="n" s="14">
+        <v>64.1838582156873</v>
+      </c>
+      <c r="G16" t="n" s="14">
+        <v>60.671234389566585</v>
+      </c>
+      <c r="H16" t="n" s="14">
+        <v>67.74065180607771</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s" s="12">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C17" t="n" s="13">
         <v>63.53225877762968</v>
@@ -1252,13 +1408,22 @@
       <c r="E17" t="n" s="13">
         <v>67.10926327299781</v>
       </c>
+      <c r="F17" t="n" s="13">
+        <v>63.19337744422458</v>
+      </c>
+      <c r="G17" t="n" s="13">
+        <v>59.68124183456188</v>
+      </c>
+      <c r="H17" t="n" s="13">
+        <v>66.7495072029777</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s" s="12">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C18" t="n" s="14">
         <v>62.54171241728688</v>
@@ -1269,13 +1434,22 @@
       <c r="E18" t="n" s="14">
         <v>66.12012808849232</v>
       </c>
+      <c r="F18" t="n" s="14">
+        <v>62.20304238244071</v>
+      </c>
+      <c r="G18" t="n" s="14">
+        <v>58.69303879956702</v>
+      </c>
+      <c r="H18" t="n" s="14">
+        <v>65.75653497937198</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s" s="12">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C19" t="n" s="13">
         <v>61.55688519324056</v>
@@ -1286,13 +1460,22 @@
       <c r="E19" t="n" s="13">
         <v>65.13458628711902</v>
       </c>
+      <c r="F19" t="n" s="13">
+        <v>61.215553843849555</v>
+      </c>
+      <c r="G19" t="n" s="13">
+        <v>57.706611420790914</v>
+      </c>
+      <c r="H19" t="n" s="13">
+        <v>64.76765380768401</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s" s="12">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C20" t="n" s="14">
         <v>60.57497331411268</v>
@@ -1303,13 +1486,22 @@
       <c r="E20" t="n" s="14">
         <v>64.14391880830853</v>
       </c>
+      <c r="F20" t="n" s="14">
+        <v>60.23786581993418</v>
+      </c>
+      <c r="G20" t="n" s="14">
+        <v>56.728755132003336</v>
+      </c>
+      <c r="H20" t="n" s="14">
+        <v>63.789937576998085</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B21" t="s" s="12">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C21" t="n" s="13">
         <v>59.594640151982055</v>
@@ -1320,13 +1512,22 @@
       <c r="E21" t="n" s="13">
         <v>63.15545682404228</v>
       </c>
+      <c r="F21" t="n" s="13">
+        <v>59.257480729153514</v>
+      </c>
+      <c r="G21" t="n" s="13">
+        <v>55.755263372158964</v>
+      </c>
+      <c r="H21" t="n" s="13">
+        <v>62.801141473907194</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s" s="12">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C22" t="n" s="14">
         <v>58.620061997406644</v>
@@ -1337,13 +1538,22 @@
       <c r="E22" t="n" s="14">
         <v>62.16914470871092</v>
       </c>
+      <c r="F22" t="n" s="14">
+        <v>58.27722977680883</v>
+      </c>
+      <c r="G22" t="n" s="14">
+        <v>54.78100080513558</v>
+      </c>
+      <c r="H22" t="n" s="14">
+        <v>61.813487709675606</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B23" t="s" s="12">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C23" t="n" s="13">
         <v>57.644362361717306</v>
@@ -1354,13 +1564,22 @@
       <c r="E23" t="n" s="13">
         <v>61.179373418264774</v>
       </c>
+      <c r="F23" t="n" s="13">
+        <v>57.30358179367205</v>
+      </c>
+      <c r="G23" t="n" s="13">
+        <v>53.81520404044189</v>
+      </c>
+      <c r="H23" t="n" s="13">
+        <v>60.83002987799322</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B24" t="s" s="12">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C24" t="n" s="14">
         <v>56.67547767552917</v>
@@ -1371,13 +1590,22 @@
       <c r="E24" t="n" s="14">
         <v>60.203574470170274</v>
       </c>
+      <c r="F24" t="n" s="14">
+        <v>56.33789579268741</v>
+      </c>
+      <c r="G24" t="n" s="14">
+        <v>52.857694379652834</v>
+      </c>
+      <c r="H24" t="n" s="14">
+        <v>59.8540980844874</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B25" t="s" s="12">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C25" t="n" s="13">
         <v>55.70861681833543</v>
@@ -1388,13 +1616,22 @@
       <c r="E25" t="n" s="13">
         <v>59.22378210558206</v>
       </c>
+      <c r="F25" t="n" s="13">
+        <v>55.37802193992169</v>
+      </c>
+      <c r="G25" t="n" s="13">
+        <v>51.9135656843771</v>
+      </c>
+      <c r="H25" t="n" s="13">
+        <v>58.87501734517949</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s" s="12">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C26" t="n" s="14">
         <v>54.734565916879696</v>
@@ -1405,13 +1642,22 @@
       <c r="E26" t="n" s="14">
         <v>58.23901562159963</v>
       </c>
+      <c r="F26" t="n" s="14">
+        <v>54.40830507151786</v>
+      </c>
+      <c r="G26" t="n" s="14">
+        <v>50.953982799792236</v>
+      </c>
+      <c r="H26" t="n" s="14">
+        <v>57.89291188033122</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s" s="12">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C27" t="n" s="13">
         <v>53.763926687175676</v>
@@ -1422,13 +1668,22 @@
       <c r="E27" t="n" s="13">
         <v>57.260605492367226</v>
       </c>
+      <c r="F27" t="n" s="13">
+        <v>53.439682319435185</v>
+      </c>
+      <c r="G27" t="n" s="13">
+        <v>49.99453379868524</v>
+      </c>
+      <c r="H27" t="n" s="13">
+        <v>56.912848342361535</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B28" t="s" s="12">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C28" t="n" s="14">
         <v>52.79244141823555</v>
@@ -1439,13 +1694,22 @@
       <c r="E28" t="n" s="14">
         <v>56.28188681468178</v>
       </c>
+      <c r="F28" t="n" s="14">
+        <v>52.46532741784809</v>
+      </c>
+      <c r="G28" t="n" s="14">
+        <v>49.03176633067459</v>
+      </c>
+      <c r="H28" t="n" s="14">
+        <v>55.92397200138737</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B29" t="s" s="12">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C29" t="n" s="13">
         <v>51.82191834772044</v>
@@ -1456,13 +1720,22 @@
       <c r="E29" t="n" s="13">
         <v>55.30345476013438</v>
       </c>
+      <c r="F29" t="n" s="13">
+        <v>51.49805873168052</v>
+      </c>
+      <c r="G29" t="n" s="13">
+        <v>48.07307294565498</v>
+      </c>
+      <c r="H29" t="n" s="13">
+        <v>54.94580317680469</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B30" t="s" s="12">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C30" t="n" s="14">
         <v>50.85992587525738</v>
@@ -1473,13 +1746,22 @@
       <c r="E30" t="n" s="14">
         <v>54.33156513822143</v>
       </c>
+      <c r="F30" t="n" s="14">
+        <v>50.53663686569379</v>
+      </c>
+      <c r="G30" t="n" s="14">
+        <v>47.12560822964408</v>
+      </c>
+      <c r="H30" t="n" s="14">
+        <v>53.966983205717554</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B31" t="s" s="12">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C31" t="n" s="13">
         <v>49.89333425967405</v>
@@ -1490,13 +1772,22 @@
       <c r="E31" t="n" s="13">
         <v>53.349805449233955</v>
       </c>
+      <c r="F31" t="n" s="13">
+        <v>49.57166578372825</v>
+      </c>
+      <c r="G31" t="n" s="13">
+        <v>46.177822069676466</v>
+      </c>
+      <c r="H31" t="n" s="13">
+        <v>52.980745212711234</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B32" t="s" s="12">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C32" t="n" s="14">
         <v>48.9254022520938</v>
@@ -1507,13 +1798,22 @@
       <c r="E32" t="n" s="14">
         <v>52.36804294131882</v>
       </c>
+      <c r="F32" t="n" s="14">
+        <v>48.600659488432015</v>
+      </c>
+      <c r="G32" t="n" s="14">
+        <v>45.21685202455385</v>
+      </c>
+      <c r="H32" t="n" s="14">
+        <v>51.99708430721393</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B33" t="s" s="12">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C33" t="n" s="13">
         <v>47.96011893361308</v>
@@ -1524,13 +1824,22 @@
       <c r="E33" t="n" s="13">
         <v>51.38908757492853</v>
       </c>
+      <c r="F33" t="n" s="13">
+        <v>47.63355076571319</v>
+      </c>
+      <c r="G33" t="n" s="13">
+        <v>44.26166387709102</v>
+      </c>
+      <c r="H33" t="n" s="13">
+        <v>51.01488759957389</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B34" t="s" s="12">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C34" t="n" s="14">
         <v>46.99816755770506</v>
@@ -1541,13 +1850,22 @@
       <c r="E34" t="n" s="14">
         <v>50.41585794684191</v>
       </c>
+      <c r="F34" t="n" s="14">
+        <v>46.66800919081846</v>
+      </c>
+      <c r="G34" t="n" s="14">
+        <v>43.29994389830548</v>
+      </c>
+      <c r="H34" t="n" s="14">
+        <v>50.044149356900206</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B35" t="s" s="12">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C35" t="n" s="13">
         <v>46.03393336376564</v>
@@ -1558,13 +1876,22 @@
       <c r="E35" t="n" s="13">
         <v>49.43599891490232</v>
       </c>
+      <c r="F35" t="n" s="13">
+        <v>45.70381351354716</v>
+      </c>
+      <c r="G35" t="n" s="13">
+        <v>42.34791224378902</v>
+      </c>
+      <c r="H35" t="n" s="13">
+        <v>49.06457742030471</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B36" t="s" s="12">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C36" t="n" s="14">
         <v>45.072386681015274</v>
@@ -1575,13 +1902,22 @@
       <c r="E36" t="n" s="14">
         <v>48.45647314597238</v>
       </c>
+      <c r="F36" t="n" s="14">
+        <v>44.737680564555745</v>
+      </c>
+      <c r="G36" t="n" s="14">
+        <v>41.39387332055868</v>
+      </c>
+      <c r="H36" t="n" s="14">
+        <v>48.08311315653352</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B37" t="s" s="12">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C37" t="n" s="13">
         <v>44.11186370948077</v>
@@ -1592,13 +1928,22 @@
       <c r="E37" t="n" s="13">
         <v>47.48011044045839</v>
       </c>
+      <c r="F37" t="n" s="13">
+        <v>43.77371233627517</v>
+      </c>
+      <c r="G37" t="n" s="13">
+        <v>40.43667087696995</v>
+      </c>
+      <c r="H37" t="n" s="13">
+        <v>47.110198979040945</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B38" t="s" s="12">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C38" t="n" s="14">
         <v>43.15439108988489</v>
@@ -1609,13 +1954,22 @@
       <c r="E38" t="n" s="14">
         <v>46.50936388799322</v>
       </c>
+      <c r="F38" t="n" s="14">
+        <v>42.81548927575815</v>
+      </c>
+      <c r="G38" t="n" s="14">
+        <v>39.49270013474346</v>
+      </c>
+      <c r="H38" t="n" s="14">
+        <v>46.1336908989468</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B39" t="s" s="12">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C39" t="n" s="13">
         <v>42.20422113804284</v>
@@ -1626,13 +1980,22 @@
       <c r="E39" t="n" s="13">
         <v>45.53629657030389</v>
       </c>
+      <c r="F39" t="n" s="13">
+        <v>41.861918744812904</v>
+      </c>
+      <c r="G39" t="n" s="13">
+        <v>38.55418518927652</v>
+      </c>
+      <c r="H39" t="n" s="13">
+        <v>45.160649869477275</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B40" t="s" s="12">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C40" t="n" s="14">
         <v>41.25032622914477</v>
@@ -1643,13 +2006,22 @@
       <c r="E40" t="n" s="14">
         <v>44.56616917777507</v>
       </c>
+      <c r="F40" t="n" s="14">
+        <v>40.908573230370465</v>
+      </c>
+      <c r="G40" t="n" s="14">
+        <v>37.61415004459598</v>
+      </c>
+      <c r="H40" t="n" s="14">
+        <v>44.189694181062244</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B41" t="s" s="12">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C41" t="n" s="13">
         <v>40.30488686582821</v>
@@ -1660,13 +2032,22 @@
       <c r="E41" t="n" s="13">
         <v>43.61068978323829</v>
       </c>
+      <c r="F41" t="n" s="13">
+        <v>39.96348646498615</v>
+      </c>
+      <c r="G41" t="n" s="13">
+        <v>36.6784507964525</v>
+      </c>
+      <c r="H41" t="n" s="13">
+        <v>43.231533935915586</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B42" t="s" s="12">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C42" t="n" s="14">
         <v>39.35641190881599</v>
@@ -1677,13 +2058,22 @@
       <c r="E42" t="n" s="14">
         <v>42.650488102195055</v>
       </c>
+      <c r="F42" t="n" s="14">
+        <v>39.014753879149886</v>
+      </c>
+      <c r="G42" t="n" s="14">
+        <v>35.73991330869649</v>
+      </c>
+      <c r="H42" t="n" s="14">
+        <v>42.26868941382356</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B43" t="s" s="12">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="C43" t="n" s="13">
         <v>38.421304818390325</v>
@@ -1694,13 +2084,22 @@
       <c r="E43" t="n" s="13">
         <v>41.69402000889223</v>
       </c>
+      <c r="F43" t="n" s="13">
+        <v>38.08326908382978</v>
+      </c>
+      <c r="G43" t="n" s="13">
+        <v>34.82450575075445</v>
+      </c>
+      <c r="H43" t="n" s="13">
+        <v>41.31501180993856</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B44" t="s" s="12">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C44" t="n" s="14">
         <v>37.483292081531324</v>
@@ -1711,13 +2110,22 @@
       <c r="E44" t="n" s="14">
         <v>40.73586684339064</v>
       </c>
+      <c r="F44" t="n" s="14">
+        <v>37.145787193258734</v>
+      </c>
+      <c r="G44" t="n" s="14">
+        <v>33.9047181215606</v>
+      </c>
+      <c r="H44" t="n" s="14">
+        <v>40.35326095021699</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B45" t="s" s="12">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="C45" t="n" s="13">
         <v>36.552668092743</v>
@@ -1728,13 +2136,22 @@
       <c r="E45" t="n" s="13">
         <v>39.78630955230102</v>
       </c>
+      <c r="F45" t="n" s="13">
+        <v>36.21112342792332</v>
+      </c>
+      <c r="G45" t="n" s="13">
+        <v>32.98648848030903</v>
+      </c>
+      <c r="H45" t="n" s="13">
+        <v>39.39584314711925</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B46" t="s" s="12">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="C46" t="n" s="14">
         <v>35.63154218222588</v>
@@ -1745,13 +2162,22 @@
       <c r="E46" t="n" s="14">
         <v>38.84666254494633</v>
       </c>
+      <c r="F46" t="n" s="14">
+        <v>35.29120491883032</v>
+      </c>
+      <c r="G46" t="n" s="14">
+        <v>32.081935147416274</v>
+      </c>
+      <c r="H46" t="n" s="14">
+        <v>38.45415088574527</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B47" t="s" s="12">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="C47" t="n" s="13">
         <v>34.70932054113482</v>
@@ -1762,13 +2188,22 @@
       <c r="E47" t="n" s="13">
         <v>37.897891603478</v>
       </c>
+      <c r="F47" t="n" s="13">
+        <v>34.368660648411435</v>
+      </c>
+      <c r="G47" t="n" s="13">
+        <v>31.17686642966408</v>
+      </c>
+      <c r="H47" t="n" s="13">
+        <v>37.50729536510975</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B48" t="s" s="12">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C48" t="n" s="14">
         <v>33.796647983160874</v>
@@ -1779,13 +2214,22 @@
       <c r="E48" t="n" s="14">
         <v>36.96176922884076</v>
       </c>
+      <c r="F48" t="n" s="14">
+        <v>33.45845352085401</v>
+      </c>
+      <c r="G48" t="n" s="14">
+        <v>30.283464536433303</v>
+      </c>
+      <c r="H48" t="n" s="14">
+        <v>36.57322270862508</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B49" t="s" s="12">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C49" t="n" s="13">
         <v>32.88166806599483</v>
@@ -1796,13 +2240,22 @@
       <c r="E49" t="n" s="13">
         <v>36.024136741729556</v>
       </c>
+      <c r="F49" t="n" s="13">
+        <v>32.5399009406097</v>
+      </c>
+      <c r="G49" t="n" s="13">
+        <v>29.378751018459063</v>
+      </c>
+      <c r="H49" t="n" s="13">
+        <v>35.6345914093493</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B50" t="s" s="12">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C50" t="n" s="14">
         <v>31.973595120026197</v>
@@ -1813,13 +2266,22 @@
       <c r="E50" t="n" s="14">
         <v>35.09592566437037</v>
       </c>
+      <c r="F50" t="n" s="14">
+        <v>31.636442504161003</v>
+      </c>
+      <c r="G50" t="n" s="14">
+        <v>28.49469589850816</v>
+      </c>
+      <c r="H50" t="n" s="14">
+        <v>34.703312718037</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B51" t="s" s="12">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C51" t="n" s="13">
         <v>31.076315457273793</v>
@@ -1830,13 +2292,22 @@
       <c r="E51" t="n" s="13">
         <v>34.16999210812367</v>
       </c>
+      <c r="F51" t="n" s="13">
+        <v>30.74688208201929</v>
+      </c>
+      <c r="G51" t="n" s="13">
+        <v>27.631187201404714</v>
+      </c>
+      <c r="H51" t="n" s="13">
+        <v>33.77701589550305</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B52" t="s" s="12">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C52" t="n" s="14">
         <v>30.18946739943648</v>
@@ -1847,13 +2318,22 @@
       <c r="E52" t="n" s="14">
         <v>33.24972337657359</v>
       </c>
+      <c r="F52" t="n" s="14">
+        <v>29.855029237214133</v>
+      </c>
+      <c r="G52" t="n" s="14">
+        <v>26.76285652561481</v>
+      </c>
+      <c r="H52" t="n" s="14">
+        <v>32.85162998155334</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B53" t="s" s="12">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C53" t="n" s="13">
         <v>29.316613008258738</v>
@@ -1864,13 +2344,22 @@
       <c r="E53" t="n" s="13">
         <v>32.333963956013356</v>
       </c>
+      <c r="F53" t="n" s="13">
+        <v>28.976241172040243</v>
+      </c>
+      <c r="G53" t="n" s="13">
+        <v>25.90965298291861</v>
+      </c>
+      <c r="H53" t="n" s="13">
+        <v>31.93560373895688</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B54" t="s" s="12">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="C54" t="n" s="14">
         <v>28.45253525919031</v>
@@ -1881,13 +2370,22 @@
       <c r="E54" t="n" s="14">
         <v>31.41927669337405</v>
       </c>
+      <c r="F54" t="n" s="14">
+        <v>28.112184341115206</v>
+      </c>
+      <c r="G54" t="n" s="14">
+        <v>25.082260205626156</v>
+      </c>
+      <c r="H54" t="n" s="14">
+        <v>31.01884017405903</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B55" t="s" s="12">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C55" t="n" s="13">
         <v>27.606480748011904</v>
@@ -1898,13 +2396,22 @@
       <c r="E55" t="n" s="13">
         <v>30.525418132518936</v>
       </c>
+      <c r="F55" t="n" s="13">
+        <v>27.268895337395627</v>
+      </c>
+      <c r="G55" t="n" s="13">
+        <v>24.270799672119324</v>
+      </c>
+      <c r="H55" t="n" s="13">
+        <v>30.128293682353544</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B56" t="s" s="12">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C56" t="n" s="14">
         <v>26.75731553492977</v>
@@ -1915,13 +2422,22 @@
       <c r="E56" t="n" s="14">
         <v>29.632245585407993</v>
       </c>
+      <c r="F56" t="n" s="14">
+        <v>26.420921080997697</v>
+      </c>
+      <c r="G56" t="n" s="14">
+        <v>23.454289884861925</v>
+      </c>
+      <c r="H56" t="n" s="14">
+        <v>29.23399568665348</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B57" t="s" s="12">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C57" t="n" s="13">
         <v>25.923472682766334</v>
@@ -1932,13 +2448,22 @@
       <c r="E57" t="n" s="13">
         <v>28.741968699031844</v>
       </c>
+      <c r="F57" t="n" s="13">
+        <v>25.574830065009778</v>
+      </c>
+      <c r="G57" t="n" s="13">
+        <v>22.644147073418278</v>
+      </c>
+      <c r="H57" t="n" s="13">
+        <v>28.336143811784925</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B58" t="s" s="12">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C58" t="n" s="14">
         <v>25.107206451632415</v>
@@ -1949,13 +2474,22 @@
       <c r="E58" t="n" s="14">
         <v>27.860906116333858</v>
       </c>
+      <c r="F58" t="n" s="14">
+        <v>24.74451896331323</v>
+      </c>
+      <c r="G58" t="n" s="14">
+        <v>21.851459331896354</v>
+      </c>
+      <c r="H58" t="n" s="14">
+        <v>27.451172352833627</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B59" t="s" s="12">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C59" t="n" s="13">
         <v>24.298813835450378</v>
@@ -1966,13 +2500,22 @@
       <c r="E59" t="n" s="13">
         <v>26.982490263283907</v>
       </c>
+      <c r="F59" t="n" s="13">
+        <v>23.924273351174197</v>
+      </c>
+      <c r="G59" t="n" s="13">
+        <v>21.081679221170777</v>
+      </c>
+      <c r="H59" t="n" s="13">
+        <v>26.55944459760832</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B60" t="s" s="12">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="C60" t="n" s="14">
         <v>23.499638391996683</v>
@@ -1983,13 +2526,22 @@
       <c r="E60" t="n" s="14">
         <v>26.117593427522156</v>
       </c>
+      <c r="F60" t="n" s="14">
+        <v>23.11870460126459</v>
+      </c>
+      <c r="G60" t="n" s="14">
+        <v>20.32123734227712</v>
+      </c>
+      <c r="H60" t="n" s="14">
+        <v>25.689074651222143</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B61" t="s" s="12">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C61" t="n" s="13">
         <v>22.71994532030395</v>
@@ -2000,13 +2552,22 @@
       <c r="E61" t="n" s="13">
         <v>25.261305558395538</v>
       </c>
+      <c r="F61" t="n" s="13">
+        <v>22.33013677468048</v>
+      </c>
+      <c r="G61" t="n" s="13">
+        <v>19.584218460178224</v>
+      </c>
+      <c r="H61" t="n" s="13">
+        <v>24.82717292599524</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B62" t="s" s="12">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C62" t="n" s="14">
         <v>21.952248024889588</v>
@@ -2017,13 +2578,22 @@
       <c r="E62" t="n" s="14">
         <v>24.411631692334097</v>
       </c>
+      <c r="F62" t="n" s="14">
+        <v>21.559443784863642</v>
+      </c>
+      <c r="G62" t="n" s="14">
+        <v>18.872548634886158</v>
+      </c>
+      <c r="H62" t="n" s="14">
+        <v>23.973411846744977</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B63" t="s" s="12">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="C63" t="n" s="13">
         <v>21.195386616515727</v>
@@ -2034,13 +2604,22 @@
       <c r="E63" t="n" s="13">
         <v>23.57371558298392</v>
       </c>
+      <c r="F63" t="n" s="13">
+        <v>20.806368761884166</v>
+      </c>
+      <c r="G63" t="n" s="13">
+        <v>18.183791883350935</v>
+      </c>
+      <c r="H63" t="n" s="13">
+        <v>23.131038027570767</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B64" t="s" s="12">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C64" t="n" s="14">
         <v>20.45004615698292</v>
@@ -2051,13 +2630,22 @@
       <c r="E64" t="n" s="14">
         <v>22.741545334730098</v>
       </c>
+      <c r="F64" t="n" s="14">
+        <v>20.050860841447346</v>
+      </c>
+      <c r="G64" t="n" s="14">
+        <v>17.49191940056443</v>
+      </c>
+      <c r="H64" t="n" s="14">
+        <v>22.287553932167757</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B65" t="s" s="12">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="C65" t="n" s="13">
         <v>19.715092623663093</v>
@@ -2068,13 +2656,22 @@
       <c r="E65" t="n" s="13">
         <v>21.930860931924347</v>
       </c>
+      <c r="F65" t="n" s="13">
+        <v>19.30931001820076</v>
+      </c>
+      <c r="G65" t="n" s="13">
+        <v>16.80235280793709</v>
+      </c>
+      <c r="H65" t="n" s="13">
+        <v>21.47202445443371</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B66" t="s" s="12">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C66" t="n" s="14">
         <v>18.98056561347593</v>
@@ -2085,13 +2682,22 @@
       <c r="E66" t="n" s="14">
         <v>21.10911006704287</v>
       </c>
+      <c r="F66" t="n" s="14">
+        <v>18.579460832890017</v>
+      </c>
+      <c r="G66" t="n" s="14">
+        <v>16.134386069967178</v>
+      </c>
+      <c r="H66" t="n" s="14">
+        <v>20.657314487816652</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B67" t="s" s="12">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C67" t="n" s="13">
         <v>18.271592157509644</v>
@@ -2102,13 +2708,22 @@
       <c r="E67" t="n" s="13">
         <v>20.30402910574062</v>
       </c>
+      <c r="F67" t="n" s="13">
+        <v>17.867947088094425</v>
+      </c>
+      <c r="G67" t="n" s="13">
+        <v>15.491280659774949</v>
+      </c>
+      <c r="H67" t="n" s="13">
+        <v>19.85442718611495</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B68" t="s" s="12">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C68" t="n" s="14">
         <v>17.578278886170605</v>
@@ -2119,13 +2734,22 @@
       <c r="E68" t="n" s="14">
         <v>19.50314761970236</v>
       </c>
+      <c r="F68" t="n" s="14">
+        <v>17.1644775838708</v>
+      </c>
+      <c r="G68" t="n" s="14">
+        <v>14.866766880315529</v>
+      </c>
+      <c r="H68" t="n" s="14">
+        <v>19.04898829235317</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B69" t="s" s="12">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="C69" t="n" s="13">
         <v>16.88063866896862</v>
@@ -2136,13 +2760,22 @@
       <c r="E69" t="n" s="13">
         <v>18.703528645081786</v>
       </c>
+      <c r="F69" t="n" s="13">
+        <v>16.46196968907437</v>
+      </c>
+      <c r="G69" t="n" s="13">
+        <v>14.241832866526726</v>
+      </c>
+      <c r="H69" t="n" s="13">
+        <v>18.24835604344572</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B70" t="s" s="12">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="C70" t="n" s="14">
         <v>16.196294862801118</v>
@@ -2153,13 +2786,22 @@
       <c r="E70" t="n" s="14">
         <v>17.919320036599288</v>
       </c>
+      <c r="F70" t="n" s="14">
+        <v>15.772500485287198</v>
+      </c>
+      <c r="G70" t="n" s="14">
+        <v>13.637306530123698</v>
+      </c>
+      <c r="H70" t="n" s="14">
+        <v>17.45452990360213</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B71" t="s" s="12">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C71" t="n" s="13">
         <v>15.52017533565187</v>
@@ -2170,13 +2812,22 @@
       <c r="E71" t="n" s="13">
         <v>17.131659730278354</v>
       </c>
+      <c r="F71" t="n" s="13">
+        <v>15.13675574767575</v>
+      </c>
+      <c r="G71" t="n" s="13">
+        <v>13.095192638507795</v>
+      </c>
+      <c r="H71" t="n" s="13">
+        <v>16.71986046610412</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B72" t="s" s="12">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="C72" t="n" s="14">
         <v>14.850001327977068</v>
@@ -2187,13 +2838,22 @@
       <c r="E72" t="n" s="14">
         <v>16.35899095084985</v>
       </c>
+      <c r="F72" t="n" s="14">
+        <v>14.514454381220537</v>
+      </c>
+      <c r="G72" t="n" s="14">
+        <v>12.57063729780749</v>
+      </c>
+      <c r="H72" t="n" s="14">
+        <v>15.995789792543917</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B73" t="s" s="12">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="C73" t="n" s="13">
         <v>14.202479677846945</v>
@@ -2204,13 +2864,22 @@
       <c r="E73" t="n" s="13">
         <v>15.597000791263527</v>
       </c>
+      <c r="F73" t="n" s="13">
+        <v>13.899095973488294</v>
+      </c>
+      <c r="G73" t="n" s="13">
+        <v>12.056198203358573</v>
+      </c>
+      <c r="H73" t="n" s="13">
+        <v>15.278539150615835</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B74" t="s" s="12">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="C74" t="n" s="14">
         <v>13.560140668839908</v>
@@ -2221,13 +2890,22 @@
       <c r="E74" t="n" s="14">
         <v>14.848790791126607</v>
       </c>
+      <c r="F74" t="n" s="14">
+        <v>13.2997127116847</v>
+      </c>
+      <c r="G74" t="n" s="14">
+        <v>11.557926750963315</v>
+      </c>
+      <c r="H74" t="n" s="14">
+        <v>14.58024790183508</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B75" t="s" s="12">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C75" t="n" s="13">
         <v>12.904391241199033</v>
@@ -2238,13 +2916,22 @@
       <c r="E75" t="n" s="13">
         <v>14.090387592092942</v>
       </c>
+      <c r="F75" t="n" s="13">
+        <v>12.703926836133633</v>
+      </c>
+      <c r="G75" t="n" s="13">
+        <v>11.068219996153745</v>
+      </c>
+      <c r="H75" t="n" s="13">
+        <v>13.883643684955459</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B76" t="s" s="12">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="C76" t="n" s="14">
         <v>12.262289529196698</v>
@@ -2255,13 +2942,22 @@
       <c r="E76" t="n" s="14">
         <v>13.35998705852937</v>
       </c>
+      <c r="F76" t="n" s="14">
+        <v>12.097324701548066</v>
+      </c>
+      <c r="G76" t="n" s="14">
+        <v>10.561757676297304</v>
+      </c>
+      <c r="H76" t="n" s="14">
+        <v>13.184870419490567</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B77" t="s" s="12">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="C77" t="n" s="13">
         <v>11.6377163549697</v>
@@ -2272,13 +2968,22 @@
       <c r="E77" t="n" s="13">
         <v>12.635038054195247</v>
       </c>
+      <c r="F77" t="n" s="13">
+        <v>11.499069671878392</v>
+      </c>
+      <c r="G77" t="n" s="13">
+        <v>10.077195565484095</v>
+      </c>
+      <c r="H77" t="n" s="13">
+        <v>12.485703189792053</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B78" t="s" s="12">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="C78" t="n" s="14">
         <v>11.02516083345175</v>
@@ -2289,13 +2994,22 @@
       <c r="E78" t="n" s="14">
         <v>11.926971181064767</v>
       </c>
+      <c r="F78" t="n" s="14">
+        <v>10.913963417586011</v>
+      </c>
+      <c r="G78" t="n" s="14">
+        <v>9.593218284343699</v>
+      </c>
+      <c r="H78" t="n" s="14">
+        <v>11.81330149872451</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B79" t="s" s="12">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="C79" t="n" s="13">
         <v>10.404255595007237</v>
@@ -2306,13 +3020,22 @@
       <c r="E79" t="n" s="13">
         <v>11.218918835048107</v>
       </c>
+      <c r="F79" t="n" s="13">
+        <v>10.343126972982814</v>
+      </c>
+      <c r="G79" t="n" s="13">
+        <v>9.129753053679966</v>
+      </c>
+      <c r="H79" t="n" s="13">
+        <v>11.152195855612952</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B80" t="s" s="12">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C80" t="n" s="14">
         <v>9.806882780390632</v>
@@ -2323,13 +3046,22 @@
       <c r="E80" t="n" s="14">
         <v>10.53659570354239</v>
       </c>
+      <c r="F80" t="n" s="14">
+        <v>9.766076475219132</v>
+      </c>
+      <c r="G80" t="n" s="14">
+        <v>8.645499646152441</v>
+      </c>
+      <c r="H80" t="n" s="14">
+        <v>10.500145598241724</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B81" t="s" s="12">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C81" t="n" s="13">
         <v>9.232476927794568</v>
@@ -2340,13 +3072,22 @@
       <c r="E81" t="n" s="13">
         <v>9.876115504824313</v>
       </c>
+      <c r="F81" t="n" s="13">
+        <v>9.221127226820013</v>
+      </c>
+      <c r="G81" t="n" s="13">
+        <v>8.209034245174713</v>
+      </c>
+      <c r="H81" t="n" s="13">
+        <v>9.869974067193533</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B82" t="s" s="12">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C82" t="n" s="14">
         <v>8.667322199924941</v>
@@ -2357,13 +3098,22 @@
       <c r="E82" t="n" s="14">
         <v>9.23836605402454</v>
       </c>
+      <c r="F82" t="n" s="14">
+        <v>8.686481500554919</v>
+      </c>
+      <c r="G82" t="n" s="14">
+        <v>7.768517899153085</v>
+      </c>
+      <c r="H82" t="n" s="14">
+        <v>9.264050089200977</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B83" t="s" s="12">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="C83" t="n" s="13">
         <v>8.1226168427521</v>
@@ -2374,13 +3124,22 @@
       <c r="E83" t="n" s="13">
         <v>8.625358536365551</v>
       </c>
+      <c r="F83" t="n" s="13">
+        <v>8.159919631259195</v>
+      </c>
+      <c r="G83" t="n" s="13">
+        <v>7.323448505660997</v>
+      </c>
+      <c r="H83" t="n" s="13">
+        <v>8.677774814590816</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B84" t="s" s="12">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C84" t="n" s="14">
         <v>7.587809250479579</v>
@@ -2391,13 +3150,22 @@
       <c r="E84" t="n" s="14">
         <v>8.034108401703781</v>
       </c>
+      <c r="F84" t="n" s="14">
+        <v>7.642978554662465</v>
+      </c>
+      <c r="G84" t="n" s="14">
+        <v>6.892483399001101</v>
+      </c>
+      <c r="H84" t="n" s="14">
+        <v>8.099614590914408</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B85" t="s" s="12">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="C85" t="n" s="13">
         <v>7.077148261415175</v>
@@ -2408,13 +3176,22 @@
       <c r="E85" t="n" s="13">
         <v>7.468086301779009</v>
       </c>
+      <c r="F85" t="n" s="13">
+        <v>7.155355316499569</v>
+      </c>
+      <c r="G85" t="n" s="13">
+        <v>6.482122139520727</v>
+      </c>
+      <c r="H85" t="n" s="13">
+        <v>7.558976469306432</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B86" t="s" s="12">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="C86" t="n" s="14">
         <v>6.596580163933073</v>
@@ -2425,13 +3202,22 @@
       <c r="E86" t="n" s="14">
         <v>6.933514590309017</v>
       </c>
+      <c r="F86" t="n" s="14">
+        <v>6.662174569336734</v>
+      </c>
+      <c r="G86" t="n" s="14">
+        <v>6.052103764529071</v>
+      </c>
+      <c r="H86" t="n" s="14">
+        <v>7.019993661622936</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B87" t="s" s="12">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="C87" t="n" s="13">
         <v>6.150430114309901</v>
@@ -2442,13 +3228,22 @@
       <c r="E87" t="n" s="13">
         <v>6.438714128415941</v>
       </c>
+      <c r="F87" t="n" s="13">
+        <v>6.206849980973817</v>
+      </c>
+      <c r="G87" t="n" s="13">
+        <v>5.666777752019885</v>
+      </c>
+      <c r="H87" t="n" s="13">
+        <v>6.516239987501698</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B88" t="s" s="12">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="C88" t="n" s="14">
         <v>5.721260460216176</v>
@@ -2459,13 +3254,22 @@
       <c r="E88" t="n" s="14">
         <v>5.9651999965729665</v>
       </c>
+      <c r="F88" t="n" s="14">
+        <v>5.77721415764944</v>
+      </c>
+      <c r="G88" t="n" s="14">
+        <v>5.30190845700791</v>
+      </c>
+      <c r="H88" t="n" s="14">
+        <v>6.043222806109338</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B89" t="s" s="12">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="C89" t="n" s="13">
         <v>5.315051457447736</v>
@@ -2476,13 +3280,22 @@
       <c r="E89" t="n" s="13">
         <v>5.5268351508451845</v>
       </c>
+      <c r="F89" t="n" s="13">
+        <v>5.368840347836855</v>
+      </c>
+      <c r="G89" t="n" s="13">
+        <v>4.9533242009241</v>
+      </c>
+      <c r="H89" t="n" s="13">
+        <v>5.595974394809296</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B90" t="s" s="12">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="C90" t="n" s="14">
         <v>4.943254929210168</v>
@@ -2493,13 +3306,22 @@
       <c r="E90" t="n" s="14">
         <v>5.130307295570702</v>
       </c>
+      <c r="F90" t="n" s="14">
+        <v>4.989466087347786</v>
+      </c>
+      <c r="G90" t="n" s="14">
+        <v>4.631941208021746</v>
+      </c>
+      <c r="H90" t="n" s="14">
+        <v>5.180012906057696</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B91" t="s" s="12">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="C91" t="n" s="13">
         <v>4.585014569101381</v>
@@ -2510,13 +3332,22 @@
       <c r="E91" t="n" s="13">
         <v>4.7445417203283755</v>
       </c>
+      <c r="F91" t="n" s="13">
+        <v>4.63669060332612</v>
+      </c>
+      <c r="G91" t="n" s="13">
+        <v>4.305956503518485</v>
+      </c>
+      <c r="H91" t="n" s="13">
+        <v>4.809255580942099</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B92" t="s" s="12">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="C92" t="n" s="14">
         <v>4.244883378506743</v>
@@ -2527,13 +3358,22 @@
       <c r="E92" t="n" s="14">
         <v>4.375969791030363</v>
       </c>
+      <c r="F92" t="n" s="14">
+        <v>4.300319901324838</v>
+      </c>
+      <c r="G92" t="n" s="14">
+        <v>4.013660443525354</v>
+      </c>
+      <c r="H92" t="n" s="14">
+        <v>4.444797215279843</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B93" t="s" s="12">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="C93" t="n" s="13">
         <v>3.919939835789004</v>
@@ -2544,13 +3384,22 @@
       <c r="E93" t="n" s="13">
         <v>4.024890871359245</v>
       </c>
+      <c r="F93" t="n" s="13">
+        <v>3.961108726958544</v>
+      </c>
+      <c r="G93" t="n" s="13">
+        <v>3.6947111851536154</v>
+      </c>
+      <c r="H93" t="n" s="13">
+        <v>4.09137059331537</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B94" t="s" s="12">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="C94" t="n" s="14">
         <v>3.619025820401608</v>
@@ -2561,13 +3410,22 @@
       <c r="E94" t="n" s="14">
         <v>3.7222780833861786</v>
       </c>
+      <c r="F94" t="n" s="14">
+        <v>3.6492262958302994</v>
+      </c>
+      <c r="G94" t="n" s="14">
+        <v>3.3842453430761146</v>
+      </c>
+      <c r="H94" t="n" s="14">
+        <v>3.775050168584454</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B95" t="s" s="12">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="C95" t="n" s="13">
         <v>3.3406797025084876</v>
@@ -2578,13 +3436,22 @@
       <c r="E95" t="n" s="13">
         <v>3.415772493947299</v>
       </c>
+      <c r="F95" t="n" s="13">
+        <v>3.3719946354980053</v>
+      </c>
+      <c r="G95" t="n" s="13">
+        <v>3.1517524942469484</v>
+      </c>
+      <c r="H95" t="n" s="13">
+        <v>3.4682313326527914</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B96" t="s" s="12">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="C96" t="n" s="14">
         <v>3.0976018110437464</v>
@@ -2595,13 +3462,22 @@
       <c r="E96" t="n" s="14">
         <v>3.1606981238208536</v>
       </c>
+      <c r="F96" t="n" s="14">
+        <v>3.1189828676168925</v>
+      </c>
+      <c r="G96" t="n" s="14">
+        <v>2.9247899855034087</v>
+      </c>
+      <c r="H96" t="n" s="14">
+        <v>3.1962181016348388</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B97" t="s" s="12">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="C97" t="n" s="13">
         <v>2.8734084098098154</v>
@@ -2612,13 +3488,22 @@
       <c r="E97" t="n" s="13">
         <v>2.9365812563709004</v>
       </c>
+      <c r="F97" t="n" s="13">
+        <v>2.8731291801527394</v>
+      </c>
+      <c r="G97" t="n" s="13">
+        <v>2.6583621524333774</v>
+      </c>
+      <c r="H97" t="n" s="13">
+        <v>2.9546180118050707</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B98" t="s" s="12">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="C98" t="n" s="14">
         <v>2.680297294010157</v>
@@ -2629,13 +3514,22 @@
       <c r="E98" t="n" s="14">
         <v>2.73570065809385</v>
       </c>
+      <c r="F98" t="n" s="14">
+        <v>2.6692374241427173</v>
+      </c>
+      <c r="G98" t="n" s="14">
+        <v>2.46328380308021</v>
+      </c>
+      <c r="H98" t="n" s="14">
+        <v>2.7380128958168855</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B99" t="s" s="12">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="C99" t="n" s="13">
         <v>2.495861051941414</v>
@@ -2646,13 +3540,22 @@
       <c r="E99" t="n" s="13">
         <v>2.5469096423756965</v>
       </c>
+      <c r="F99" t="n" s="13">
+        <v>2.4946628643473283</v>
+      </c>
+      <c r="G99" t="n" s="13">
+        <v>2.2135821459993243</v>
+      </c>
+      <c r="H99" t="n" s="13">
+        <v>2.5433533812286098</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B100" t="s" s="12">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="C100" t="n" s="14">
         <v>2.281207346532171</v>
@@ -2663,13 +3566,22 @@
       <c r="E100" t="n" s="14">
         <v>2.324532225594613</v>
       </c>
+      <c r="F100" t="n" s="14">
+        <v>2.282355430449854</v>
+      </c>
+      <c r="G100" t="n" s="14">
+        <v>2.036324475554767</v>
+      </c>
+      <c r="H100" t="n" s="14">
+        <v>2.3241167751132954</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B101" t="s" s="12">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="C101" t="n" s="13">
         <v>2.0766227887483217</v>
@@ -2680,13 +3592,22 @@
       <c r="E101" t="n" s="13">
         <v>2.1297381449151915</v>
       </c>
+      <c r="F101" t="n" s="13">
+        <v>2.0720021476305828</v>
+      </c>
+      <c r="G101" t="n" s="13">
+        <v>1.8731041336083534</v>
+      </c>
+      <c r="H101" t="n" s="13">
+        <v>2.113450761215455</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B102" t="s" s="12">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C102" t="n" s="14">
         <v>1.8165577147759115</v>
@@ -2697,13 +3618,22 @@
       <c r="E102" t="n" s="14">
         <v>1.8865680668327764</v>
       </c>
+      <c r="F102" t="n" s="14">
+        <v>1.8369408965774892</v>
+      </c>
+      <c r="G102" t="n" s="14">
+        <v>1.6870807470011482</v>
+      </c>
+      <c r="H102" t="n" s="14">
+        <v>1.8700236805733208</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B103" t="s" s="12">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="C103" t="n" s="13">
         <v>1.5172008177858256</v>
@@ -2714,13 +3644,22 @@
       <c r="E103" t="n" s="13">
         <v>1.5851981262437815</v>
       </c>
+      <c r="F103" t="n" s="13">
+        <v>1.5002788979784023</v>
+      </c>
+      <c r="G103" t="n" s="13">
+        <v>1.4381070867753993</v>
+      </c>
+      <c r="H103" t="n" s="13">
+        <v>1.5372395515253217</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B104" t="s" s="12">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="C104" t="n" s="14">
         <v>1.102757299815618</v>
@@ -2731,13 +3670,22 @@
       <c r="E104" t="n" s="14">
         <v>1.1425571688011626</v>
       </c>
+      <c r="F104" t="n" s="14">
+        <v>1.0981720670280826</v>
+      </c>
+      <c r="G104" t="n" s="14">
+        <v>1.0663579622011743</v>
+      </c>
+      <c r="H104" t="n" s="14">
+        <v>1.1081767894851178</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="s" s="11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B105" t="s" s="12">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="C105" t="n" s="13">
         <v>0.4756791632054179</v>
@@ -2748,20 +3696,29 @@
       <c r="E105" t="n" s="13">
         <v>0.4790886392009987</v>
       </c>
+      <c r="F105" t="n" s="13">
+        <v>0.47529456480425697</v>
+      </c>
+      <c r="G105" t="n" s="13">
+        <v>0.4721784618414266</v>
+      </c>
+      <c r="H105" t="n" s="13">
+        <v>0.47613458528951486</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="s" s="2">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s" s="2">
-        <v>216</v>
+        <v>222</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s" s="3">
-        <v>217</v>
+        <v>223</v>
       </c>
     </row>
     <row r="111">
@@ -2769,7 +3726,7 @@
         <v>0</v>
       </c>
       <c r="B111" t="s" s="3">
-        <v>218</v>
+        <v>224</v>
       </c>
     </row>
     <row r="112">
@@ -2777,7 +3734,7 @@
         <v>0</v>
       </c>
       <c r="B112" t="s" s="3">
-        <v>219</v>
+        <v>225</v>
       </c>
     </row>
     <row r="113">
@@ -2785,12 +3742,12 @@
         <v>0</v>
       </c>
       <c r="B113" t="s" s="3">
-        <v>220</v>
+        <v>226</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s" s="3">
-        <v>221</v>
+        <v>227</v>
       </c>
     </row>
     <row r="115">
@@ -2798,7 +3755,7 @@
         <v>0</v>
       </c>
       <c r="B115" t="s" s="3">
-        <v>222</v>
+        <v>228</v>
       </c>
     </row>
     <row r="116">
@@ -2806,18 +3763,20 @@
         <v>0</v>
       </c>
       <c r="B116" t="s" s="3">
-        <v>223</v>
+        <v>229</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s" s="3">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
     <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A5:A105"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>